<commit_message>
Added 1 more test case espn
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/espnFootBallTestData.xlsx
+++ b/com.espn/src/test/resources/espnFootBallTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janna\IdeaProjects\Team1BootCamp\com.espn\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417FFBD1-B148-41D6-8F22-3409CC90EA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79005DA-55B1-430C-A82B-10BD3B7DA1F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7785" yWindow="2925" windowWidth="18435" windowHeight="11385" firstSheet="1" activeTab="4" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Table" sheetId="6" r:id="rId3"/>
     <sheet name="TableColoumnNames" sheetId="7" r:id="rId4"/>
     <sheet name="EnglishPremiumLeaguePosition" sheetId="8" r:id="rId5"/>
-    <sheet name="OverStock" sheetId="9" r:id="rId6"/>
+    <sheet name="YearResult" sheetId="9" r:id="rId6"/>
     <sheet name="ESPN" sheetId="10" r:id="rId7"/>
     <sheet name="Verizon" sheetId="11" r:id="rId8"/>
     <sheet name="Chase" sheetId="12" r:id="rId9"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Category Name</t>
   </si>
@@ -179,6 +179,69 @@
   </si>
   <si>
     <t>Position 5: Europa League</t>
+  </si>
+  <si>
+    <t>YearResult</t>
+  </si>
+  <si>
+    <t>2021-22</t>
+  </si>
+  <si>
+    <t>2020-21</t>
+  </si>
+  <si>
+    <t>2019-20</t>
+  </si>
+  <si>
+    <t>2018-19</t>
+  </si>
+  <si>
+    <t>2017-18</t>
+  </si>
+  <si>
+    <t>2016-17</t>
+  </si>
+  <si>
+    <t>2015-16</t>
+  </si>
+  <si>
+    <t>2014-15</t>
+  </si>
+  <si>
+    <t>2013-14</t>
+  </si>
+  <si>
+    <t>2012-13</t>
+  </si>
+  <si>
+    <t>2011-12</t>
+  </si>
+  <si>
+    <t>2010-11</t>
+  </si>
+  <si>
+    <t>2009-10</t>
+  </si>
+  <si>
+    <t>2008-09</t>
+  </si>
+  <si>
+    <t>2007-08</t>
+  </si>
+  <si>
+    <t>2006-07</t>
+  </si>
+  <si>
+    <t>2005-06</t>
+  </si>
+  <si>
+    <t>2004-05</t>
+  </si>
+  <si>
+    <t>2003-04</t>
+  </si>
+  <si>
+    <t>2002-03</t>
   </si>
 </sst>
 </file>
@@ -902,7 +965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F06E338-1C0F-45E0-B136-3FC6897D7CEC}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -937,12 +1000,118 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A9241A-80CA-47A8-B8A7-CE843E51095C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>